<commit_message>
changed readme, after the graph changed
</commit_message>
<xml_diff>
--- a/doc (graph)/cs313f16p2-PlotofGraph.xlsx
+++ b/doc (graph)/cs313f16p2-PlotofGraph.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyleerchinger/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyleerchinger/Documents/Comp 313/cs313f16p2/doc (graph)/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="560" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="25600" yWindow="-5140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>x= collection size</t>
   </si>
@@ -32,10 +32,16 @@
     <t>y= runtime</t>
   </si>
   <si>
-    <t>ArrayList</t>
+    <t>ArrayList Access</t>
   </si>
   <si>
-    <t>LinkedList</t>
+    <t>ArrayList Add/Remove</t>
+  </si>
+  <si>
+    <t>LinkedList Access</t>
+  </si>
+  <si>
+    <t>LinkedList Add/Remove</t>
   </si>
 </sst>
 </file>
@@ -173,7 +179,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>ArrayList</c:v>
+            <c:v>ArrayList Access</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -212,19 +218,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>138.0</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>161.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>854.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4530.0</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="#,##0">
-                  <c:v>9036.0</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -235,7 +241,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>LinkedList</c:v>
+            <c:v>ArrayList Add/Remove</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -274,19 +280,143 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>111.0</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>149.0</c:v>
+                  <c:v>59.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>758.0</c:v>
+                  <c:v>318.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4596.0</c:v>
+                  <c:v>1270.0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="#,##0">
-                  <c:v>9024.0</c:v>
+                  <c:v>3492.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>LinkedList Access</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>10.0</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>100.0</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>1000.0</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>10000.0</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$5:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>437.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2983.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6335.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>LinkedList Add/Remove</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>10.0</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>100.0</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>1000.0</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>10000.0</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$5:$M$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -302,11 +432,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2036741616"/>
-        <c:axId val="-2013073456"/>
+        <c:axId val="-2071125600"/>
+        <c:axId val="-2084380656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2036741616"/>
+        <c:axId val="-2071125600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -423,7 +553,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2013073456"/>
+        <c:crossAx val="-2084380656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -431,10 +561,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2013073456"/>
+        <c:axId val="-2084380656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="10000.0"/>
+          <c:max val="7000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -544,7 +674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2036741616"/>
+        <c:crossAx val="-2071125600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1173,15 +1303,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1466,10 +1596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:G9"/>
+  <dimension ref="C3:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1478,15 +1608,21 @@
     <col min="4" max="4" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
       </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -1499,75 +1635,147 @@
       <c r="G4" t="s">
         <v>1</v>
       </c>
+      <c r="I4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5">
         <v>10</v>
       </c>
       <c r="D5">
-        <v>138</v>
+        <v>14</v>
       </c>
       <c r="F5">
         <v>10</v>
       </c>
       <c r="G5">
-        <v>111</v>
+        <v>51</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>19</v>
+      </c>
+      <c r="L5">
+        <v>10</v>
+      </c>
+      <c r="M5">
+        <v>49</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6">
         <v>100</v>
       </c>
       <c r="D6">
-        <v>161</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>100</v>
       </c>
       <c r="G6">
-        <v>149</v>
+        <v>59</v>
+      </c>
+      <c r="I6">
+        <v>100</v>
+      </c>
+      <c r="J6">
+        <v>32</v>
+      </c>
+      <c r="L6">
+        <v>100</v>
+      </c>
+      <c r="M6">
+        <v>46</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7">
         <v>1000</v>
       </c>
       <c r="D7">
-        <v>854</v>
+        <v>11</v>
       </c>
       <c r="F7">
         <v>1000</v>
       </c>
       <c r="G7">
-        <v>758</v>
+        <v>318</v>
+      </c>
+      <c r="I7">
+        <v>1000</v>
+      </c>
+      <c r="J7">
+        <v>437</v>
+      </c>
+      <c r="L7">
+        <v>1000</v>
+      </c>
+      <c r="M7">
+        <v>45</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8">
         <v>5000</v>
       </c>
       <c r="D8">
-        <v>4530</v>
+        <v>19</v>
       </c>
       <c r="F8">
         <v>5000</v>
       </c>
       <c r="G8">
-        <v>4596</v>
+        <v>1270</v>
+      </c>
+      <c r="I8">
+        <v>5000</v>
+      </c>
+      <c r="J8">
+        <v>2983</v>
+      </c>
+      <c r="L8">
+        <v>5000</v>
+      </c>
+      <c r="M8">
+        <v>43</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9">
         <v>10000</v>
       </c>
       <c r="D9" s="1">
-        <v>9036</v>
+        <v>23</v>
       </c>
       <c r="F9">
         <v>10000</v>
       </c>
       <c r="G9" s="1">
-        <v>9024</v>
+        <v>3492</v>
+      </c>
+      <c r="I9">
+        <v>10000</v>
+      </c>
+      <c r="J9">
+        <v>6335</v>
+      </c>
+      <c r="L9">
+        <v>10000</v>
+      </c>
+      <c r="M9">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>